<commit_message>
add descriptions to tables
</commit_message>
<xml_diff>
--- a/results/tables/2025-03-23/table_s1.xlsx
+++ b/results/tables/2025-03-23/table_s1.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="description" sheetId="1" r:id="rId1"/>
+    <sheet name="table S1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -340,7 +341,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -349,6 +350,33 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Metrics are included for training, validation, and testing data. Two models were selected for each subset (GBM, DNN) based on validation metrics.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>cell_type</t>
         </is>
       </c>

</xml_diff>